<commit_message>
Modified ServiceListingVariation01.java and ProductLandingVariation6.java for wave6 fixes Modified wave6.xlsx for en_au managed cloud services 3rd column
</commit_message>
<xml_diff>
--- a/docs/Language Waves/wave6.xlsx
+++ b/docs/Language Waves/wave6.xlsx
@@ -2141,8 +2141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:D6"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2834,7 +2834,7 @@
         <v>119</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>238</v>
       </c>
       <c r="D43" t="s">
         <v>88</v>
@@ -3489,8 +3489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added wireless/technology to wave6 file
</commit_message>
<xml_diff>
--- a/docs/Language Waves/wave6.xlsx
+++ b/docs/Language Waves/wave6.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW Migration\OVWMigration\docs\Language Waves\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agarnepu\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="19140" windowHeight="7350"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="19140" windowHeight="7350" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="en_au" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2652" uniqueCount="571">
   <si>
     <t>http://www.cisco.com/web/ANZ/ordering/index.html</t>
   </si>
@@ -1737,6 +1737,15 @@
   </si>
   <si>
     <t>solutions-listing-var9</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/products/wireless/technology.html</t>
+  </si>
+  <si>
+    <t>technology-rvar2</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/products/products_netsol/wireless/technology.html</t>
   </si>
 </sst>
 </file>
@@ -2141,7 +2150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -4813,10 +4822,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93:E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6346,6 +6355,23 @@
         <v>86</v>
       </c>
       <c r="E92" s="8" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>570</v>
+      </c>
+      <c r="B93" t="s">
+        <v>133</v>
+      </c>
+      <c r="C93" t="s">
+        <v>569</v>
+      </c>
+      <c r="D93" t="s">
+        <v>86</v>
+      </c>
+      <c r="E93" s="8" t="s">
         <v>565</v>
       </c>
     </row>
@@ -9830,10 +9856,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94:E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11379,6 +11405,23 @@
         <v>565</v>
       </c>
     </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>568</v>
+      </c>
+      <c r="B94" t="s">
+        <v>133</v>
+      </c>
+      <c r="C94" t="s">
+        <v>569</v>
+      </c>
+      <c r="D94" t="s">
+        <v>86</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>565</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A39" r:id="rId1"/>

</xml_diff>

<commit_message>
Added one url in zh_cn
</commit_message>
<xml_diff>
--- a/docs/Language Waves/wave6.xlsx
+++ b/docs/Language Waves/wave6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agarnepu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW Migration\OVWMigration\docs\Language Waves\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2652" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2657" uniqueCount="572">
   <si>
     <t>http://www.cisco.com/web/ANZ/ordering/index.html</t>
   </si>
@@ -1746,6 +1746,9 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/CN/products/products_netsol/wireless/technology.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/solutions/trends/cloud/managed-cloud-services.html</t>
   </si>
 </sst>
 </file>
@@ -4822,10 +4825,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93:E93"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94:E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6372,6 +6375,23 @@
         <v>86</v>
       </c>
       <c r="E93" s="8" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>571</v>
+      </c>
+      <c r="B94" t="s">
+        <v>119</v>
+      </c>
+      <c r="C94" t="s">
+        <v>122</v>
+      </c>
+      <c r="D94" t="s">
+        <v>88</v>
+      </c>
+      <c r="E94" t="s">
         <v>565</v>
       </c>
     </row>

</xml_diff>